<commit_message>
type: feat Save the report file
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/result/detailed_results.xlsx
+++ b/POS Code/Experiments/result/detailed_results.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuh/Documents/interpretability-of-source-code-transformers/POS Code/Experiments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuh/Documents/interpretability-of-source-code-transformers/POS Code/Experiments/result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9389A92-E304-6B47-8809-42109DA541AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0367C2-B3F6-6149-A9ED-216D5BC87B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="15440" xr2:uid="{BEC22610-DBDE-49A5-ABDC-7DB261D6BA7F}"/>
+    <workbookView xWindow="20" yWindow="660" windowWidth="28800" windowHeight="15440" xr2:uid="{BEC22610-DBDE-49A5-ABDC-7DB261D6BA7F}"/>
   </bookViews>
   <sheets>
     <sheet name="POSSummary" sheetId="3" r:id="rId1"/>
     <sheet name="DefDetSummary" sheetId="6" r:id="rId2"/>
     <sheet name="POSLayerwise" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -14332,7 +14333,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18277,20 +18278,32 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D67:D79"/>
+    <mergeCell ref="I67:I79"/>
+    <mergeCell ref="N67:N79"/>
+    <mergeCell ref="D99:D111"/>
+    <mergeCell ref="I99:I111"/>
+    <mergeCell ref="N99:N111"/>
     <mergeCell ref="D2:D14"/>
     <mergeCell ref="I2:I14"/>
     <mergeCell ref="N2:N8"/>
     <mergeCell ref="D34:D46"/>
     <mergeCell ref="I34:I46"/>
     <mergeCell ref="N34:N46"/>
-    <mergeCell ref="D67:D79"/>
-    <mergeCell ref="I67:I79"/>
-    <mergeCell ref="N67:N79"/>
-    <mergeCell ref="D99:D111"/>
-    <mergeCell ref="I99:I111"/>
-    <mergeCell ref="N99:N111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD302C83-6A19-1746-8058-E37651EDB290}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
type: feat Save the summary report
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/result/detailed_results.xlsx
+++ b/POS Code/Experiments/result/detailed_results.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuh/Documents/interpretability-of-source-code-transformers/POS Code/Experiments/result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0367C2-B3F6-6149-A9ED-216D5BC87B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3F4DE2-AFDC-6844-AD3A-3B1AD5C180AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="660" windowWidth="28800" windowHeight="15440" xr2:uid="{BEC22610-DBDE-49A5-ABDC-7DB261D6BA7F}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="15440" activeTab="3" xr2:uid="{BEC22610-DBDE-49A5-ABDC-7DB261D6BA7F}"/>
   </bookViews>
   <sheets>
     <sheet name="POSSummary" sheetId="3" r:id="rId1"/>
     <sheet name="DefDetSummary" sheetId="6" r:id="rId2"/>
     <sheet name="POSLayerwise" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
+    <sheet name="CloneDetecLayerwise" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="43">
   <si>
     <t>Selection</t>
   </si>
@@ -300,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -389,6 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2568,6 +2569,1128 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="534980847"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GraphCodeBERT</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CloneDetecLayerwise!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>CloneDetecLayerwise!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CloneDetecLayerwise!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.66666700000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53886800000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54850200000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53795800000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54511100000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.54999500000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.552315</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56195499999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.57339300000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.57301899999999995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.57183899999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55879900000000005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.50923399999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8055-1341-8677-D0341DB41884}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CloneDetecLayerwise!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Incremental</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>CloneDetecLayerwise!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CloneDetecLayerwise!$C$2:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.66666700000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51964299999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54270200000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58758500000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59606400000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.63406600000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.63100100000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.62990500000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.62997499999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.629741</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.62902800000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.65797799999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.57034200000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8055-1341-8677-D0341DB41884}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="748756847"/>
+        <c:axId val="748757247"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="748756847"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="748757247"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="748757247"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="748756847"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>UniXCoder</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CloneDetecLayerwise!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>CloneDetecLayerwise!$F$2:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CloneDetecLayerwise!$G$2:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.223861</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C6A2-0D4A-9451-253FFCE7BD15}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CloneDetecLayerwise!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Incremental</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>CloneDetecLayerwise!$F$2:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CloneDetecLayerwise!$H$2:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.1979999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.66666700000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66666700000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.212117</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C6A2-0D4A-9451-253FFCE7BD15}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="749196047"/>
+        <c:axId val="752715711"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="749196047"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="752715711"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="752715711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="749196047"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7240,6 +8363,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -9070,6 +10273,1012 @@
 </file>
 
 <file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -14033,6 +16242,83 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC7258C6-C790-251B-2B0A-CE08CB0693FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6643271-4D06-4A72-8F7B-2DE129CB67EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -14332,7 +16618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1929D321-160C-41CB-828A-0FA5B23B672C}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
@@ -16497,8 +18783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F291A794-F81B-A94A-B246-9FC1326ED183}">
   <dimension ref="A1:N111"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="O130" sqref="O130"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection sqref="A1:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18278,18 +20564,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D2:D14"/>
+    <mergeCell ref="I2:I14"/>
+    <mergeCell ref="N2:N8"/>
+    <mergeCell ref="D34:D46"/>
+    <mergeCell ref="I34:I46"/>
+    <mergeCell ref="N34:N46"/>
     <mergeCell ref="D67:D79"/>
     <mergeCell ref="I67:I79"/>
     <mergeCell ref="N67:N79"/>
     <mergeCell ref="D99:D111"/>
     <mergeCell ref="I99:I111"/>
     <mergeCell ref="N99:N111"/>
-    <mergeCell ref="D2:D14"/>
-    <mergeCell ref="I2:I14"/>
-    <mergeCell ref="N2:N8"/>
-    <mergeCell ref="D34:D46"/>
-    <mergeCell ref="I34:I46"/>
-    <mergeCell ref="N34:N46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18298,12 +20584,333 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD302C83-6A19-1746-8058-E37651EDB290}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="30">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="C2" s="30">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="30">
+        <v>0</v>
+      </c>
+      <c r="H2" s="30">
+        <v>0</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30">
+        <v>0.53886800000000001</v>
+      </c>
+      <c r="C3" s="30">
+        <v>0.51964299999999997</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="30">
+        <v>0</v>
+      </c>
+      <c r="H3" s="30">
+        <v>9.1979999999999996E-3</v>
+      </c>
+      <c r="I3" s="29"/>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="30">
+        <v>0.54850200000000005</v>
+      </c>
+      <c r="C4" s="30">
+        <v>0.54270200000000002</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="30">
+        <v>0</v>
+      </c>
+      <c r="H4" s="30">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="I4" s="29"/>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="30">
+        <v>0.53795800000000005</v>
+      </c>
+      <c r="C5" s="30">
+        <v>0.58758500000000002</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="30">
+        <v>0</v>
+      </c>
+      <c r="H5" s="30">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="I5" s="29"/>
+    </row>
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="30">
+        <v>0.54511100000000001</v>
+      </c>
+      <c r="C6" s="30">
+        <v>0.59606400000000004</v>
+      </c>
+      <c r="D6" s="29"/>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="30">
+        <v>0</v>
+      </c>
+      <c r="H6" s="30">
+        <v>0</v>
+      </c>
+      <c r="I6" s="29"/>
+    </row>
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="30">
+        <v>0.54999500000000001</v>
+      </c>
+      <c r="C7" s="30">
+        <v>0.63406600000000002</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="30">
+        <v>0</v>
+      </c>
+      <c r="H7" s="30">
+        <v>0</v>
+      </c>
+      <c r="I7" s="29"/>
+    </row>
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="30">
+        <v>0.552315</v>
+      </c>
+      <c r="C8" s="30">
+        <v>0.63100100000000003</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8" s="30">
+        <v>0</v>
+      </c>
+      <c r="H8" s="30">
+        <v>0</v>
+      </c>
+      <c r="I8" s="29"/>
+    </row>
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="30">
+        <v>0.56195499999999998</v>
+      </c>
+      <c r="C9" s="30">
+        <v>0.62990500000000005</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="F9" s="1">
+        <v>7</v>
+      </c>
+      <c r="G9" s="30">
+        <v>0</v>
+      </c>
+      <c r="H9" s="30">
+        <v>0</v>
+      </c>
+      <c r="I9" s="29"/>
+    </row>
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="30">
+        <v>0.57339300000000004</v>
+      </c>
+      <c r="C10" s="30">
+        <v>0.62997499999999995</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="F10" s="1">
+        <v>8</v>
+      </c>
+      <c r="G10" s="30">
+        <v>0</v>
+      </c>
+      <c r="H10" s="30">
+        <v>0</v>
+      </c>
+      <c r="I10" s="29"/>
+    </row>
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="30">
+        <v>0.57301899999999995</v>
+      </c>
+      <c r="C11" s="30">
+        <v>0.629741</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="F11" s="1">
+        <v>9</v>
+      </c>
+      <c r="G11" s="30">
+        <v>0</v>
+      </c>
+      <c r="H11" s="30">
+        <v>0</v>
+      </c>
+      <c r="I11" s="29"/>
+    </row>
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="30">
+        <v>0.57183899999999999</v>
+      </c>
+      <c r="C12" s="30">
+        <v>0.62902800000000003</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="F12" s="1">
+        <v>10</v>
+      </c>
+      <c r="G12" s="30">
+        <v>0</v>
+      </c>
+      <c r="H12" s="30">
+        <v>0</v>
+      </c>
+      <c r="I12" s="29"/>
+    </row>
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="30">
+        <v>0.55879900000000005</v>
+      </c>
+      <c r="C13" s="30">
+        <v>0.65797799999999995</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="F13" s="1">
+        <v>11</v>
+      </c>
+      <c r="G13" s="30">
+        <v>0</v>
+      </c>
+      <c r="H13" s="30">
+        <v>0</v>
+      </c>
+      <c r="I13" s="29"/>
+    </row>
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="30">
+        <v>0.50923399999999996</v>
+      </c>
+      <c r="C14" s="30">
+        <v>0.57034200000000002</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="F14" s="1">
+        <v>12</v>
+      </c>
+      <c r="G14" s="30">
+        <v>0.223861</v>
+      </c>
+      <c r="H14" s="30">
+        <v>0.212117</v>
+      </c>
+      <c r="I14" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D2:D14"/>
+    <mergeCell ref="I2:I14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>